<commit_message>
progress made thus far
</commit_message>
<xml_diff>
--- a/center_bounds.xlsx
+++ b/center_bounds.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programs\z_PROJECTS\MCL Project\Raman-Peak-Fitting-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2499B34-A0C3-4F42-94A8-A3D440453A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8EA0FA-D885-401C-ACDA-14341FB584E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3883408C-F2D1-4228-8870-6F9136675442}"/>
   </bookViews>
@@ -406,7 +406,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,7 +437,7 @@
         <v>1106.0899999999999</v>
       </c>
       <c r="C2" s="1">
-        <f>A2+10</f>
+        <f t="shared" ref="C2:C12" si="0">A2+10</f>
         <v>1126.0899999999999</v>
       </c>
     </row>
@@ -450,7 +450,7 @@
         <v>1215.49</v>
       </c>
       <c r="C3" s="1">
-        <f>A3+10</f>
+        <f t="shared" si="0"/>
         <v>1235.49</v>
       </c>
     </row>
@@ -463,7 +463,7 @@
         <v>1341.36</v>
       </c>
       <c r="C4" s="1">
-        <f>A4+10</f>
+        <f t="shared" si="0"/>
         <v>1361.36</v>
       </c>
     </row>
@@ -476,7 +476,7 @@
         <v>1485.35</v>
       </c>
       <c r="C5" s="1">
-        <f>A5+10</f>
+        <f t="shared" si="0"/>
         <v>1505.35</v>
       </c>
     </row>
@@ -489,7 +489,7 @@
         <v>1585.8</v>
       </c>
       <c r="C6" s="1">
-        <f>A6+10</f>
+        <f t="shared" si="0"/>
         <v>1605.8</v>
       </c>
     </row>
@@ -501,7 +501,7 @@
         <v>1610</v>
       </c>
       <c r="C7" s="1">
-        <f>A7+10</f>
+        <f t="shared" si="0"/>
         <v>1638.02</v>
       </c>
     </row>
@@ -514,7 +514,7 @@
         <v>2472.39</v>
       </c>
       <c r="C8" s="1">
-        <f>A8+10</f>
+        <f t="shared" si="0"/>
         <v>2492.39</v>
       </c>
     </row>
@@ -527,7 +527,7 @@
         <v>2681.12</v>
       </c>
       <c r="C9" s="1">
-        <f>A9+10</f>
+        <f t="shared" si="0"/>
         <v>2701.12</v>
       </c>
     </row>
@@ -540,7 +540,7 @@
         <v>2930.8</v>
       </c>
       <c r="C10" s="1">
-        <f>A10+10</f>
+        <f t="shared" si="0"/>
         <v>2950.8</v>
       </c>
     </row>
@@ -553,7 +553,7 @@
         <v>3218.2</v>
       </c>
       <c r="C11" s="1">
-        <f>A11+10</f>
+        <f t="shared" si="0"/>
         <v>3238.2</v>
       </c>
     </row>
@@ -566,7 +566,7 @@
         <v>4259.25</v>
       </c>
       <c r="C12" s="1">
-        <f>A12+10</f>
+        <f t="shared" si="0"/>
         <v>4279.25</v>
       </c>
     </row>

</xml_diff>